<commit_message>
moved old versions of state data
</commit_message>
<xml_diff>
--- a/data/raw/USFWS_bull_trout_SSA_data_OR_LowCr.xlsx
+++ b/data/raw/USFWS_bull_trout_SSA_data_OR_LowCr.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\USFWS Liason\Bull Trout\5-Year Review\Data\Scheuller analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scheuerl/Documents/GitHub/bulltrout/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47732912-6EDF-49F3-821F-AE20CB059E6F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18787907-5AE2-C140-AD62-6A548D31AB0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FF99D774-9E75-4C57-897F-F0A14D004F26}"/>
+    <workbookView xWindow="1000" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{FF99D774-9E75-4C57-897F-F0A14D004F26}"/>
   </bookViews>
   <sheets>
     <sheet name="Walla Walla - Low Creek" sheetId="1" r:id="rId1"/>
+    <sheet name="metadata" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -81,7 +82,7 @@
     <t>not surveyed</t>
   </si>
   <si>
-    <t xml:space="preserve">metadata -&gt; annual redd surveys in Low Creek with experienced and consistent surveyors.  These surveys detected few if any large fluvial fish sized redds, all were resident adults.  </t>
+    <t xml:space="preserve">]annual redd surveys in Low Creek with experienced and consistent surveyors.  These surveys detected few if any large fluvial fish sized redds, all were resident adults.  </t>
   </si>
 </sst>
 </file>
@@ -467,23 +468,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D460C10-3A5B-4A2E-911A-4A2B95C3A11E}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.21875" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.109375" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -512,8 +513,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="4" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
+    <row r="2" spans="1:9" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>29</v>
+      </c>
       <c r="B2" s="4" t="s">
         <v>9</v>
       </c>
@@ -537,7 +540,10 @@
       </c>
       <c r="I2" s="7"/>
     </row>
-    <row r="3" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>29</v>
+      </c>
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
@@ -560,7 +566,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>29</v>
+      </c>
       <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
@@ -583,7 +592,10 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>29</v>
+      </c>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
@@ -606,7 +618,10 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>29</v>
+      </c>
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
@@ -629,7 +644,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>29</v>
+      </c>
       <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
@@ -652,7 +670,10 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>29</v>
+      </c>
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
@@ -675,7 +696,10 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>29</v>
+      </c>
       <c r="B9" s="4" t="s">
         <v>9</v>
       </c>
@@ -698,7 +722,10 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>29</v>
+      </c>
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
@@ -721,7 +748,10 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>29</v>
+      </c>
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
@@ -745,7 +775,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>29</v>
+      </c>
       <c r="B12" s="4" t="s">
         <v>9</v>
       </c>
@@ -768,7 +801,10 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>29</v>
+      </c>
       <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
@@ -791,7 +827,10 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>29</v>
+      </c>
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
@@ -814,8 +853,23 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CFA7A20-3AD8-5346-9615-CEDD7330205B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed colnames for raw data
</commit_message>
<xml_diff>
--- a/data/raw/USFWS_bull_trout_SSA_data_OR_LowCr.xlsx
+++ b/data/raw/USFWS_bull_trout_SSA_data_OR_LowCr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scheuerl/Documents/GitHub/bulltrout/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18787907-5AE2-C140-AD62-6A548D31AB0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8AB5313-C0F1-584D-B65D-EA144D5E9350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{FF99D774-9E75-4C57-897F-F0A14D004F26}"/>
   </bookViews>
@@ -37,33 +37,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="16">
   <si>
-    <t>Dataset</t>
-  </si>
-  <si>
-    <t>Recovery Unit</t>
-  </si>
-  <si>
-    <t>Core Area</t>
-  </si>
-  <si>
-    <t>Local Pop</t>
-  </si>
-  <si>
-    <t>Method</t>
-  </si>
-  <si>
-    <t>Metric</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Value</t>
-  </si>
-  <si>
-    <t>Data notes</t>
-  </si>
-  <si>
     <t>Mid-Columbia</t>
   </si>
   <si>
@@ -83,13 +56,40 @@
   </si>
   <si>
     <t xml:space="preserve">]annual redd surveys in Low Creek with experienced and consistent surveyors.  These surveys detected few if any large fluvial fish sized redds, all were resident adults.  </t>
+  </si>
+  <si>
+    <t>dataset</t>
+  </si>
+  <si>
+    <t>recovery unit</t>
+  </si>
+  <si>
+    <t>core area</t>
+  </si>
+  <si>
+    <t>popn/stream</t>
+  </si>
+  <si>
+    <t>metric</t>
+  </si>
+  <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>notes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -111,6 +111,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -134,12 +140,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -152,6 +154,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -470,9 +475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D460C10-3A5B-4A2E-911A-4A2B95C3A11E}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -484,85 +487,85 @@
     <col min="9" max="9" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="B1" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
-        <v>29</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="6">
+      <c r="H1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="4">
         <v>1998</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="4">
         <v>27</v>
       </c>
-      <c r="I2" s="7"/>
+      <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>29</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="6">
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="4">
         <v>1999</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="4">
         <v>41</v>
       </c>
     </row>
@@ -570,25 +573,25 @@
       <c r="A4">
         <v>29</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="6">
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="4">
         <v>2000</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="4">
         <v>39</v>
       </c>
     </row>
@@ -596,25 +599,25 @@
       <c r="A5">
         <v>29</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="6">
+      <c r="B5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="4">
         <v>2001</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="4">
         <v>33</v>
       </c>
     </row>
@@ -622,25 +625,25 @@
       <c r="A6">
         <v>29</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="6">
+      <c r="B6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="4">
         <v>2002</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="4">
         <v>32</v>
       </c>
     </row>
@@ -648,25 +651,25 @@
       <c r="A7">
         <v>29</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="6">
+      <c r="B7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="4">
         <v>2003</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="4">
         <v>28</v>
       </c>
     </row>
@@ -674,25 +677,25 @@
       <c r="A8">
         <v>29</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="6">
+      <c r="B8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="4">
         <v>2004</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="4">
         <v>61</v>
       </c>
     </row>
@@ -700,25 +703,25 @@
       <c r="A9">
         <v>29</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="6">
+      <c r="B9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="4">
         <v>2005</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="4">
         <v>43</v>
       </c>
     </row>
@@ -726,25 +729,25 @@
       <c r="A10">
         <v>29</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="6">
+      <c r="B10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="4">
         <v>2006</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="4">
         <v>35</v>
       </c>
     </row>
@@ -752,52 +755,52 @@
       <c r="A11">
         <v>29</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="6">
+      <c r="B11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="4">
         <v>2007</v>
       </c>
-      <c r="H11" s="6"/>
+      <c r="H11" s="4"/>
       <c r="I11" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>29</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" s="6">
+      <c r="B12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="4">
         <v>2008</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="4">
         <v>47</v>
       </c>
     </row>
@@ -805,25 +808,25 @@
       <c r="A13">
         <v>29</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="6">
+      <c r="B13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="4">
         <v>2009</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="4">
         <v>39</v>
       </c>
     </row>
@@ -831,25 +834,25 @@
       <c r="A14">
         <v>29</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="6">
+      <c r="B14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="4">
         <v>2010</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="4">
         <v>36</v>
       </c>
     </row>
@@ -870,7 +873,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>